<commit_message>
fix fgistExport and cadExport
</commit_message>
<xml_diff>
--- a/Defaults/p10-2024.xlsx
+++ b/Defaults/p10-2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ya.shatalov\Desktop\Data\GIS\Toolboxex\Defaults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE636E8-98B4-4BC3-9F7F-E8531152E668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66928C1C-BBD6-43BD-9546-47710F26EC78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8839,8 +8839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F99B37A-B714-4679-B3FC-AE5B06855E12}">
   <dimension ref="A1:J1581"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A628" workbookViewId="0">
-      <selection activeCell="B669" sqref="B669"/>
+    <sheetView tabSelected="1" topLeftCell="A265" workbookViewId="0">
+      <selection activeCell="F291" sqref="F291"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>